<commit_message>
updating marketing quiz spreadsheet and power point analysis
</commit_message>
<xml_diff>
--- a/Copy of Marketing Analytics Quiz.xlsx
+++ b/Copy of Marketing Analytics Quiz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/christiana_o_mensah_accenture_com/Documents/Documents/Projects/Sql-Project-Assessment/ForcastingCase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{BD547CEA-C048-4FE9-A6E8-22B6959B1BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BC3A370-DB85-4357-BE9D-2F1A63746889}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{BD547CEA-C048-4FE9-A6E8-22B6959B1BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{855DD711-BFBF-4439-A15E-DD4852A23CFA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7270" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forecasting Case " sheetId="1" r:id="rId1"/>
@@ -334,16 +334,10 @@
     <t>C) Select region, customer_Id from Customer where customer_id IN (select customer_id from Customer group by customer_id having count(distinct region)&gt;1 )</t>
   </si>
   <si>
-    <t xml:space="preserve">A) Select region, count(visit_id)  from Customer, Visit Where Customer.customer_id = Visit.customer_id  AND region  like 'North America' group by region  </t>
-  </si>
-  <si>
     <t>B) Select device, avg(visit_duration)  from Customer, Visit Where Customer.customer_id = Visit.customer_id group by device order by avg(visit_duration) desc</t>
   </si>
   <si>
     <t>C) Select device, visit_type, avg(visit_value)  from Customer, Visit Where Customer.customer_id = Visit.customer_id group by visit_type, device order by avg(visit_value), device Desc</t>
-  </si>
-  <si>
-    <t>D) Select product,  avg(visit_value)/count(customer_id)  AS "Average value per customer" from Visit group by  product order by "Average value per customer" Limit 1</t>
   </si>
   <si>
     <t xml:space="preserve">select </t>
@@ -356,6 +350,12 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A) Select region, count(visit_id)  from Customer, Visit Where Customer.customer_id = Visit.customer_id  AND region  like 'North America' AND visit_date BETWEEN '$2021-01-01' AND '$2021-12-31') group by region  </t>
+  </si>
+  <si>
+    <t>D) Select product,  sum(visit_value)/count(customer_id)  AS "Average value per customer" from Visit group by  product order by "Average value per customer" Limit 1</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>2</v>
@@ -40628,7 +40628,7 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="E16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -41773,8 +41773,8 @@
   </sheetPr>
   <dimension ref="A1:L1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -42144,24 +42144,24 @@
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="18"/>
       <c r="B28" s="48" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="18"/>
       <c r="B29" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="18"/>
       <c r="B30" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="B31" s="49" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
@@ -42176,13 +42176,13 @@
     <row r="34" spans="1:2" ht="15.75" customHeight="1">
       <c r="A34" s="18"/>
       <c r="B34" s="29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1">
       <c r="A35" s="18"/>
       <c r="B35" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1">
@@ -42191,7 +42191,7 @@
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1">
       <c r="B37" s="44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
@@ -43198,15 +43198,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A6A93819D24DA4439E53B03368A1DFB7" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e173a0fc61e51b4fff85c97566ffd9b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6f4ecc09-967a-4a46-a8d0-e4b5aae47e48" xmlns:ns4="707d8c2f-4129-478b-9349-8e9edb14722d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fac0b6fe56baecc663d99a1c1d718bcd" ns3:_="" ns4:_="">
     <xsd:import namespace="6f4ecc09-967a-4a46-a8d0-e4b5aae47e48"/>
@@ -43459,6 +43450,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -43473,14 +43473,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F0516E6-A8B2-444A-B736-9A3D5FCCAEB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D49615-7890-46E2-8452-746617AA67D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43495,6 +43487,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F0516E6-A8B2-444A-B736-9A3D5FCCAEB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>